<commit_message>
added independent variables beyond sex
</commit_message>
<xml_diff>
--- a/Data/AcomysDomRegen_Inventory.xlsx
+++ b/Data/AcomysDomRegen_Inventory.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive-105793286447324059497/My Drive/RStudio/Dominance Project/DomRegen_Data_Repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinvarholick/Documents/GitHub/AcomysDominance_2022_Data_Results/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0850E95A-35E0-F649-A49E-4CD8BCD182D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12CCFF12-73B4-704C-9728-5517128AFFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16860" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
+    <workbookView xWindow="38400" yWindow="9260" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="sexes" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="85">
   <si>
     <t>CageID</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>OF</t>
+  </si>
+  <si>
+    <t>GrpSize</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Young</t>
   </si>
 </sst>
 </file>
@@ -691,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548C978-8C0A-483F-BBE8-CAC5FEF0E8F4}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -2258,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88D8F42-D426-4BA6-AEB8-A4D66EEEB1BD}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
@@ -3176,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5C8D93-7AE0-4EA0-BF68-EDDEB9ED6B6E}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3187,111 +3199,189 @@
     <col min="1" max="1" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>957162</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922587</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>941702</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>927693</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>990342</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1001363</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>1064394</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>1062366</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>1068572</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>1074455</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>1058108</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>925878</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised for manu rewrite 1.1
</commit_message>
<xml_diff>
--- a/Data/AcomysDomRegen_Inventory.xlsx
+++ b/Data/AcomysDomRegen_Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinvarholick/Documents/GitHub/AcomysDominance_2022_Data_Results/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0117E3-0892-0948-AE44-3A5B689D8851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD65BC-D382-144A-BB59-FFAD2942AEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19320" yWindow="0" windowWidth="19080" windowHeight="21600" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
+    <workbookView xWindow="9660" yWindow="0" windowWidth="19080" windowHeight="21600" activeTab="2" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="85">
   <si>
     <t>CageID</t>
   </si>
@@ -269,15 +269,6 @@
     <t>Trt</t>
   </si>
   <si>
-    <t>YF</t>
-  </si>
-  <si>
-    <t>YM</t>
-  </si>
-  <si>
-    <t>OF</t>
-  </si>
-  <si>
     <t>GrpSize</t>
   </si>
   <si>
@@ -288,6 +279,18 @@
   </si>
   <si>
     <t>Young</t>
+  </si>
+  <si>
+    <t>YFD</t>
+  </si>
+  <si>
+    <t>YMT</t>
+  </si>
+  <si>
+    <t>YMD</t>
+  </si>
+  <si>
+    <t>OFD</t>
   </si>
 </sst>
 </file>
@@ -700,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548C978-8C0A-483F-BBE8-CAC5FEF0E8F4}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -729,7 +732,7 @@
         <v>76</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1</v>
@@ -776,7 +779,7 @@
         <v>957162</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
@@ -832,7 +835,7 @@
         <v>957162</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -885,7 +888,7 @@
         <v>922587</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -938,7 +941,7 @@
         <v>922587</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -991,7 +994,7 @@
         <v>941702</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -1044,7 +1047,7 @@
         <v>941702</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -1097,7 +1100,7 @@
         <v>941702</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -1150,7 +1153,7 @@
         <v>927693</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -1203,7 +1206,7 @@
         <v>927693</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -1256,7 +1259,7 @@
         <v>1064394</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D11" s="10">
         <v>2</v>
@@ -1310,7 +1313,7 @@
         <v>1064394</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
@@ -1369,7 +1372,7 @@
         <v>1062366</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D13" s="10">
         <v>2</v>
@@ -1428,7 +1431,7 @@
         <v>1062366</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D14" s="10">
         <v>2</v>
@@ -1487,7 +1490,7 @@
         <v>1068572</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D15" s="10">
         <v>3</v>
@@ -1546,7 +1549,7 @@
         <v>1068572</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D16" s="10">
         <v>3</v>
@@ -1605,7 +1608,7 @@
         <v>1068572</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D17" s="10">
         <v>3</v>
@@ -1664,7 +1667,7 @@
         <v>1074455</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D18" s="10">
         <v>2</v>
@@ -1723,7 +1726,7 @@
         <v>1074455</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D19" s="10">
         <v>2</v>
@@ -1782,7 +1785,7 @@
         <v>1058108</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D20" s="10">
         <v>3</v>
@@ -1841,7 +1844,7 @@
         <v>1058108</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D21" s="10">
         <v>3</v>
@@ -1900,7 +1903,7 @@
         <v>1058108</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D22" s="10">
         <v>3</v>
@@ -1959,7 +1962,7 @@
         <v>925878</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -2010,7 +2013,7 @@
         <v>925878</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D24" s="13">
         <v>2</v>
@@ -2063,7 +2066,7 @@
         <v>990342</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D25" s="13">
         <v>2</v>
@@ -2114,7 +2117,7 @@
         <v>990342</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D26" s="13">
         <v>2</v>
@@ -2162,7 +2165,7 @@
         <v>1001363</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -2210,7 +2213,7 @@
         <v>1001363</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D28" s="13">
         <v>2</v>
@@ -3179,10 +3182,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5C8D93-7AE0-4EA0-BF68-EDDEB9ED6B6E}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3190,7 +3193,7 @@
     <col min="1" max="1" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>66</v>
       </c>
@@ -3198,13 +3201,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>957162</v>
       </c>
@@ -3215,10 +3221,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922587</v>
       </c>
@@ -3229,10 +3238,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>941702</v>
       </c>
@@ -3243,10 +3255,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>927693</v>
       </c>
@@ -3257,10 +3272,13 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>990342</v>
       </c>
@@ -3271,10 +3289,13 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1001363</v>
       </c>
@@ -3285,10 +3306,13 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>1064394</v>
       </c>
@@ -3299,10 +3323,13 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>1062366</v>
       </c>
@@ -3313,10 +3340,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>1068572</v>
       </c>
@@ -3327,10 +3357,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>1074455</v>
       </c>
@@ -3341,10 +3374,13 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>1058108</v>
       </c>
@@ -3355,10 +3391,13 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>925878</v>
       </c>
@@ -3369,10 +3408,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Age is primary effect
</commit_message>
<xml_diff>
--- a/Data/AcomysDomRegen_Inventory.xlsx
+++ b/Data/AcomysDomRegen_Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinvarholick/Documents/GitHub/AcomysDominance_2022_Data_Results/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD65BC-D382-144A-BB59-FFAD2942AEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7392D666-B516-0A44-B1E4-0D411A2CDFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="0" windowWidth="19080" windowHeight="21600" activeTab="2" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{25090408-5A55-4AED-BABD-C45A2B3F66DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="86">
   <si>
     <t>CageID</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>OFD</t>
+  </si>
+  <si>
+    <t>dpi</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -380,7 +383,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -701,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548C978-8C0A-483F-BBE8-CAC5FEF0E8F4}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -719,9 +721,10 @@
     <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -770,8 +773,11 @@
       <c r="P1" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -823,11 +829,15 @@
         <f t="shared" ref="P2:P10" si="2">(M2-I2)/365</f>
         <v>0.75890410958904109</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="4">
+        <f>M2-K2</f>
+        <v>119</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -879,8 +889,12 @@
         <f t="shared" si="2"/>
         <v>0.75890410958904109</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q28" si="3">M3-K3</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -932,8 +946,12 @@
         <f t="shared" si="2"/>
         <v>1.1041095890410959</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q4" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -985,8 +1003,12 @@
         <f t="shared" si="2"/>
         <v>1.1041095890410959</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q5" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1038,8 +1060,12 @@
         <f t="shared" si="2"/>
         <v>0.92328767123287669</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1091,8 +1117,12 @@
         <f t="shared" si="2"/>
         <v>0.9068493150684932</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q7" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1144,8 +1174,12 @@
         <f t="shared" si="2"/>
         <v>0.87123287671232874</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q8" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1197,8 +1231,12 @@
         <f t="shared" si="2"/>
         <v>1.0547945205479452</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q9" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1250,1008 +1288,1029 @@
         <f t="shared" si="2"/>
         <v>1.0547945205479452</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="Q10" s="4">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>1064394</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="10">
-        <v>2</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
         <v>22</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>43991</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>44012</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>44109</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="11">
         <v>45.9</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>44175</v>
       </c>
-      <c r="N11" s="10">
-        <f t="shared" ref="N11" si="3">J11-I11</f>
+      <c r="N11" s="9">
+        <f t="shared" ref="N11" si="4">J11-I11</f>
         <v>21</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <f>K11-I11</f>
         <v>118</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="11">
         <f>(M11-I11)/365</f>
         <v>0.50410958904109593</v>
       </c>
-      <c r="Q11" s="10"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="Q11" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R11" s="9"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>1064394</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="10">
-        <v>2</v>
-      </c>
-      <c r="E12" s="10">
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9">
         <v>26</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>43991</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <v>44012</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <v>44109</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="11">
         <v>45</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <v>44175</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" ref="N12:N28" si="4">J12-I12</f>
+      <c r="N12" s="9">
+        <f t="shared" ref="N12:N28" si="5">J12-I12</f>
         <v>21</v>
       </c>
-      <c r="O12" s="10">
-        <f t="shared" ref="O12:O28" si="5">K12-I12</f>
+      <c r="O12" s="9">
+        <f t="shared" ref="O12:O28" si="6">K12-I12</f>
         <v>118</v>
       </c>
-      <c r="P12" s="12">
-        <f t="shared" ref="P12:P25" si="6">(M12-I12)/365</f>
+      <c r="P12" s="11">
+        <f t="shared" ref="P12:P25" si="7">(M12-I12)/365</f>
         <v>0.50410958904109593</v>
       </c>
-      <c r="Q12" s="10"/>
+      <c r="Q12" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
       <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>1062366</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="10">
-        <v>2</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
         <v>18</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>43972</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <v>44000</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <v>44109</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <v>48.8</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="10">
         <v>44175</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="4"/>
+      <c r="N13" s="9">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
+        <f t="shared" si="6"/>
+        <v>137</v>
+      </c>
+      <c r="P13" s="11">
+        <f t="shared" si="7"/>
+        <v>0.55616438356164388</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1062366</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>18</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="10">
+        <v>43972</v>
+      </c>
+      <c r="J14" s="10">
+        <v>44000</v>
+      </c>
+      <c r="K14" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L14" s="11">
+        <v>42.2</v>
+      </c>
+      <c r="M14" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N14" s="9">
         <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="O14" s="9">
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P14" s="11">
+        <f t="shared" si="7"/>
+        <v>0.55616438356164388</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1068572</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="E15" s="9">
+        <v>24</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="10">
+        <v>44001</v>
+      </c>
+      <c r="J15" s="10">
+        <v>44033</v>
+      </c>
+      <c r="K15" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L15" s="11">
+        <v>42.8</v>
+      </c>
+      <c r="M15" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N15" s="9">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="O15" s="9">
         <f t="shared" si="6"/>
-        <v>0.55616438356164388</v>
-      </c>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" s="11">
+        <f t="shared" si="7"/>
+        <v>0.47671232876712327</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R15" s="9"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="10">
-        <v>1062366</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="10">
-        <v>2</v>
-      </c>
-      <c r="E14" s="10">
+      <c r="B16" s="9">
+        <v>1068572</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="9">
+        <v>3</v>
+      </c>
+      <c r="E16" s="9">
+        <v>23</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="10">
+        <v>44010</v>
+      </c>
+      <c r="J16" s="10">
+        <v>44033</v>
+      </c>
+      <c r="K16" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L16" s="11">
+        <v>44.4</v>
+      </c>
+      <c r="M16" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+      <c r="P16" s="11">
+        <f t="shared" si="7"/>
+        <v>0.45205479452054792</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R16" s="9"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1068572</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="9">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9">
         <v>18</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="10" t="s">
+      <c r="F17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="11">
-        <v>43972</v>
-      </c>
-      <c r="J14" s="11">
-        <v>44000</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="I17" s="10">
+        <v>44011</v>
+      </c>
+      <c r="J17" s="10">
+        <v>44033</v>
+      </c>
+      <c r="K17" s="10">
         <v>44109</v>
       </c>
-      <c r="L14" s="12">
-        <v>42.2</v>
-      </c>
-      <c r="M14" s="11">
+      <c r="L17" s="11">
+        <v>41.3</v>
+      </c>
+      <c r="M17" s="10">
         <v>44175</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="O14" s="10">
+      <c r="N17" s="9">
         <f t="shared" si="5"/>
-        <v>137</v>
-      </c>
-      <c r="P14" s="12">
+        <v>22</v>
+      </c>
+      <c r="O17" s="9">
         <f t="shared" si="6"/>
-        <v>0.55616438356164388</v>
-      </c>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="P17" s="11">
+        <f t="shared" si="7"/>
+        <v>0.44931506849315067</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R17" s="9"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="10">
-        <v>1068572</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B18" s="9">
+        <v>1074455</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9">
+        <v>994804</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="10">
+        <v>44021</v>
+      </c>
+      <c r="J18" s="10">
+        <v>44056</v>
+      </c>
+      <c r="K18" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L18" s="11">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="M18" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N18" s="9">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="O18" s="9">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="P18" s="11">
+        <f t="shared" si="7"/>
+        <v>0.42191780821917807</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1074455</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>26</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="10">
+        <v>44021</v>
+      </c>
+      <c r="J19" s="10">
+        <v>44056</v>
+      </c>
+      <c r="K19" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L19" s="11">
+        <v>42.7</v>
+      </c>
+      <c r="M19" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N19" s="9">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="P19" s="11">
+        <f t="shared" si="7"/>
+        <v>0.42191780821917807</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R19" s="9"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1058108</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="10">
-        <v>3</v>
-      </c>
-      <c r="E15" s="10">
-        <v>24</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="10" t="s">
+      <c r="D20" s="9">
+        <v>3</v>
+      </c>
+      <c r="E20" s="9">
+        <v>853839</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="11">
-        <v>44001</v>
-      </c>
-      <c r="J15" s="11">
-        <v>44033</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="I20" s="10">
+        <v>43934</v>
+      </c>
+      <c r="J20" s="10">
+        <v>43971</v>
+      </c>
+      <c r="K20" s="10">
         <v>44109</v>
       </c>
-      <c r="L15" s="12">
-        <v>42.8</v>
-      </c>
-      <c r="M15" s="11">
+      <c r="L20" s="11">
+        <v>45.9</v>
+      </c>
+      <c r="M20" s="10">
         <v>44175</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="O15" s="10">
+      <c r="N20" s="9">
         <f t="shared" si="5"/>
-        <v>108</v>
-      </c>
-      <c r="P15" s="12">
+        <v>37</v>
+      </c>
+      <c r="O20" s="9">
         <f t="shared" si="6"/>
-        <v>0.47671232876712327</v>
-      </c>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="P20" s="11">
+        <f t="shared" si="7"/>
+        <v>0.66027397260273968</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R20" s="9"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="10">
-        <v>1068572</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B21" s="9">
+        <v>1058108</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="10">
-        <v>3</v>
-      </c>
-      <c r="E16" s="10">
+      <c r="D21" s="9">
+        <v>3</v>
+      </c>
+      <c r="E21" s="9">
+        <v>853839</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="10">
+        <v>43934</v>
+      </c>
+      <c r="J21" s="10">
+        <v>43971</v>
+      </c>
+      <c r="K21" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L21" s="11">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="M21" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N21" s="9">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="O21" s="9">
+        <f t="shared" si="6"/>
+        <v>175</v>
+      </c>
+      <c r="P21" s="11">
+        <f t="shared" si="7"/>
+        <v>0.66027397260273968</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R21" s="9"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1058108</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="9">
+        <v>3</v>
+      </c>
+      <c r="E22" s="9">
+        <v>853839</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="10">
+        <v>43934</v>
+      </c>
+      <c r="J22" s="10">
+        <v>43971</v>
+      </c>
+      <c r="K22" s="10">
+        <v>44109</v>
+      </c>
+      <c r="L22" s="11">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="M22" s="10">
+        <v>44175</v>
+      </c>
+      <c r="N22" s="9">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="O22" s="9">
+        <f t="shared" si="6"/>
+        <v>175</v>
+      </c>
+      <c r="P22" s="11">
+        <f t="shared" si="7"/>
+        <v>0.66027397260273968</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="R22" s="9"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="11">
-        <v>44010</v>
-      </c>
-      <c r="J16" s="11">
-        <v>44033</v>
-      </c>
-      <c r="K16" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L16" s="12">
-        <v>44.4</v>
-      </c>
-      <c r="M16" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N16" s="10">
-        <f t="shared" si="4"/>
+      <c r="B23" s="12">
+        <v>925878</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="13">
+        <v>42852</v>
+      </c>
+      <c r="J23" s="13">
+        <v>42879</v>
+      </c>
+      <c r="K23" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L23" s="14">
+        <v>51.2</v>
+      </c>
+      <c r="M23" s="13">
+        <v>43877</v>
+      </c>
+      <c r="N23" s="12">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="O23" s="12">
+        <f t="shared" si="6"/>
+        <v>1021</v>
+      </c>
+      <c r="P23" s="14">
+        <f t="shared" si="7"/>
+        <v>2.8082191780821919</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="O16" s="10">
+      <c r="B24" s="12">
+        <v>925878</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2</v>
+      </c>
+      <c r="E24" s="12">
+        <v>11</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="13">
+        <v>42852</v>
+      </c>
+      <c r="J24" s="13">
+        <v>42879</v>
+      </c>
+      <c r="K24" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L24" s="14">
+        <v>54.2</v>
+      </c>
+      <c r="M24" s="13">
+        <v>43877</v>
+      </c>
+      <c r="N24" s="12">
         <f t="shared" si="5"/>
-        <v>99</v>
-      </c>
-      <c r="P16" s="12">
+        <v>27</v>
+      </c>
+      <c r="O24" s="12">
         <f t="shared" si="6"/>
-        <v>0.45205479452054792</v>
-      </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="10">
-        <v>1068572</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="10">
-        <v>3</v>
-      </c>
-      <c r="E17" s="10">
-        <v>18</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="11">
-        <v>44011</v>
-      </c>
-      <c r="J17" s="11">
-        <v>44033</v>
-      </c>
-      <c r="K17" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L17" s="12">
-        <v>41.3</v>
-      </c>
-      <c r="M17" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N17" s="10">
-        <f t="shared" si="4"/>
+        <v>1021</v>
+      </c>
+      <c r="P24" s="14">
+        <f t="shared" si="7"/>
+        <v>2.8082191780821919</v>
+      </c>
+      <c r="Q24" s="4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="12">
+        <v>990342</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="12">
+        <v>2</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="13">
+        <v>43167</v>
+      </c>
+      <c r="J25" s="13">
+        <v>43188</v>
+      </c>
+      <c r="K25" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L25" s="14">
+        <v>44.6</v>
+      </c>
+      <c r="M25" s="13">
+        <v>43958</v>
+      </c>
+      <c r="N25" s="12">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="12">
+        <f t="shared" si="6"/>
+        <v>706</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" si="7"/>
+        <v>2.1671232876712327</v>
+      </c>
+      <c r="Q25" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="12">
+        <v>990342</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="12">
+        <v>2</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="13">
+        <v>43167</v>
+      </c>
+      <c r="J26" s="13">
+        <v>43188</v>
+      </c>
+      <c r="K26" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L26" s="14">
+        <v>41.6</v>
+      </c>
+      <c r="M26" s="13">
+        <v>43958</v>
+      </c>
+      <c r="N26" s="12">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="O26" s="12">
+        <f t="shared" si="6"/>
+        <v>706</v>
+      </c>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1001363</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="12">
+        <v>2</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="13">
+        <v>42829</v>
+      </c>
+      <c r="J27" s="13">
+        <v>42850</v>
+      </c>
+      <c r="K27" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L27" s="14">
+        <v>46.8</v>
+      </c>
+      <c r="M27" s="13">
+        <v>43958</v>
+      </c>
+      <c r="N27" s="12">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="O27" s="12">
+        <f t="shared" si="6"/>
+        <v>1044</v>
+      </c>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="12">
+        <v>1001363</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="12">
+        <v>2</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="13">
+        <v>42829</v>
+      </c>
+      <c r="J28" s="13">
+        <v>42851</v>
+      </c>
+      <c r="K28" s="13">
+        <v>43873</v>
+      </c>
+      <c r="L28" s="14">
+        <v>54.1</v>
+      </c>
+      <c r="M28" s="13">
+        <v>43958</v>
+      </c>
+      <c r="N28" s="12">
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="O17" s="10">
-        <f t="shared" si="5"/>
-        <v>98</v>
-      </c>
-      <c r="P17" s="12">
+      <c r="O28" s="12">
         <f t="shared" si="6"/>
-        <v>0.44931506849315067</v>
-      </c>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="10">
-        <v>1074455</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="10">
-        <v>2</v>
-      </c>
-      <c r="E18" s="10">
-        <v>994804</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="11">
-        <v>44021</v>
-      </c>
-      <c r="J18" s="11">
-        <v>44056</v>
-      </c>
-      <c r="K18" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L18" s="12">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="M18" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N18" s="10">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="O18" s="10">
-        <f t="shared" si="5"/>
-        <v>88</v>
-      </c>
-      <c r="P18" s="12">
-        <f t="shared" si="6"/>
-        <v>0.42191780821917807</v>
-      </c>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="10">
-        <v>1074455</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="10">
-        <v>2</v>
-      </c>
-      <c r="E19" s="10">
-        <v>26</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="11">
-        <v>44021</v>
-      </c>
-      <c r="J19" s="11">
-        <v>44056</v>
-      </c>
-      <c r="K19" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L19" s="12">
-        <v>42.7</v>
-      </c>
-      <c r="M19" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N19" s="10">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="O19" s="10">
-        <f t="shared" si="5"/>
-        <v>88</v>
-      </c>
-      <c r="P19" s="12">
-        <f t="shared" si="6"/>
-        <v>0.42191780821917807</v>
-      </c>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="10">
-        <v>1058108</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="10">
-        <v>3</v>
-      </c>
-      <c r="E20" s="10">
-        <v>853839</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="11">
-        <v>43934</v>
-      </c>
-      <c r="J20" s="11">
-        <v>43971</v>
-      </c>
-      <c r="K20" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L20" s="12">
-        <v>45.9</v>
-      </c>
-      <c r="M20" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N20" s="10">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="O20" s="10">
-        <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-      <c r="P20" s="12">
-        <f t="shared" si="6"/>
-        <v>0.66027397260273968</v>
-      </c>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="10">
-        <v>1058108</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="10">
-        <v>3</v>
-      </c>
-      <c r="E21" s="10">
-        <v>853839</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="11">
-        <v>43934</v>
-      </c>
-      <c r="J21" s="11">
-        <v>43971</v>
-      </c>
-      <c r="K21" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L21" s="12">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="M21" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N21" s="10">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="O21" s="10">
-        <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-      <c r="P21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.66027397260273968</v>
-      </c>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="10">
-        <v>1058108</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="10">
-        <v>3</v>
-      </c>
-      <c r="E22" s="10">
-        <v>853839</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="11">
-        <v>43934</v>
-      </c>
-      <c r="J22" s="11">
-        <v>43971</v>
-      </c>
-      <c r="K22" s="11">
-        <v>44109</v>
-      </c>
-      <c r="L22" s="12">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="M22" s="11">
-        <v>44175</v>
-      </c>
-      <c r="N22" s="10">
-        <f t="shared" si="4"/>
-        <v>37</v>
-      </c>
-      <c r="O22" s="10">
-        <f t="shared" si="5"/>
-        <v>175</v>
-      </c>
-      <c r="P22" s="12">
-        <f t="shared" si="6"/>
-        <v>0.66027397260273968</v>
-      </c>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="13">
-        <v>925878</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="13">
-        <v>2</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" s="14">
-        <v>42852</v>
-      </c>
-      <c r="J23" s="14">
-        <v>42879</v>
-      </c>
-      <c r="K23" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L23" s="15">
-        <v>51.2</v>
-      </c>
-      <c r="M23" s="14">
-        <v>43877</v>
-      </c>
-      <c r="N23" s="13">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="O23" s="13">
-        <f t="shared" si="5"/>
-        <v>1021</v>
-      </c>
-      <c r="P23" s="15">
-        <f t="shared" si="6"/>
-        <v>2.8082191780821919</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13">
-        <v>925878</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="13">
-        <v>2</v>
-      </c>
-      <c r="E24" s="13">
-        <v>11</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="14">
-        <v>42852</v>
-      </c>
-      <c r="J24" s="14">
-        <v>42879</v>
-      </c>
-      <c r="K24" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L24" s="15">
-        <v>54.2</v>
-      </c>
-      <c r="M24" s="14">
-        <v>43877</v>
-      </c>
-      <c r="N24" s="13">
-        <f t="shared" si="4"/>
-        <v>27</v>
-      </c>
-      <c r="O24" s="13">
-        <f t="shared" si="5"/>
-        <v>1021</v>
-      </c>
-      <c r="P24" s="15">
-        <f t="shared" si="6"/>
-        <v>2.8082191780821919</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="13">
-        <v>990342</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="13">
-        <v>2</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="14">
-        <v>43167</v>
-      </c>
-      <c r="J25" s="14">
-        <v>43188</v>
-      </c>
-      <c r="K25" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L25" s="15">
-        <v>44.6</v>
-      </c>
-      <c r="M25" s="14">
-        <v>43958</v>
-      </c>
-      <c r="N25" s="13">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="O25" s="13">
-        <f t="shared" si="5"/>
-        <v>706</v>
-      </c>
-      <c r="P25" s="15">
-        <f t="shared" si="6"/>
-        <v>2.1671232876712327</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="13">
-        <v>990342</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="13">
-        <v>2</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="14">
-        <v>43167</v>
-      </c>
-      <c r="J26" s="14">
-        <v>43188</v>
-      </c>
-      <c r="K26" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L26" s="15">
-        <v>41.6</v>
-      </c>
-      <c r="M26" s="14">
-        <v>43958</v>
-      </c>
-      <c r="N26" s="13">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="O26" s="13">
-        <f t="shared" si="5"/>
-        <v>706</v>
-      </c>
-      <c r="P26" s="15"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="13">
-        <v>1001363</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="13">
-        <v>2</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="14">
-        <v>42829</v>
-      </c>
-      <c r="J27" s="14">
-        <v>42850</v>
-      </c>
-      <c r="K27" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L27" s="15">
-        <v>46.8</v>
-      </c>
-      <c r="M27" s="14">
-        <v>43958</v>
-      </c>
-      <c r="N27" s="13">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="O27" s="13">
-        <f t="shared" si="5"/>
         <v>1044</v>
       </c>
-      <c r="P27" s="15"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="13">
-        <v>1001363</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="13">
-        <v>2</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="14">
-        <v>42829</v>
-      </c>
-      <c r="J28" s="14">
-        <v>42851</v>
-      </c>
-      <c r="K28" s="14">
-        <v>43873</v>
-      </c>
-      <c r="L28" s="15">
-        <v>54.1</v>
-      </c>
-      <c r="M28" s="14">
-        <v>43958</v>
-      </c>
-      <c r="N28" s="13">
-        <f t="shared" si="4"/>
-        <v>22</v>
-      </c>
-      <c r="O28" s="13">
-        <f t="shared" si="5"/>
-        <v>1044</v>
-      </c>
-      <c r="P28" s="15"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2428,10 +2487,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>1064394</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C15">
@@ -2439,10 +2498,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>1064394</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C16">
@@ -2450,10 +2509,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>1062366</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C17">
@@ -2461,10 +2520,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>1062366</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C18">
@@ -2472,10 +2531,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>1068572</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C19">
@@ -2483,10 +2542,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>1068572</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C20">
@@ -2494,10 +2553,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>1068572</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C21">
@@ -2505,10 +2564,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>1074455</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C22">
@@ -2516,10 +2575,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>1074455</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C23">
@@ -2527,10 +2586,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>1058108</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C24">
@@ -2538,10 +2597,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>1058108</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C25">
@@ -2549,10 +2608,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>1058108</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C26">
@@ -2703,10 +2762,10 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>1064394</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C40">
@@ -2714,10 +2773,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>1064394</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C41">
@@ -2725,10 +2784,10 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <v>1062366</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C42">
@@ -2736,10 +2795,10 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <v>1062366</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C43">
@@ -2747,10 +2806,10 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>1068572</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C44">
@@ -2758,10 +2817,10 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>1068572</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C45">
@@ -2769,10 +2828,10 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="10">
+      <c r="A46" s="9">
         <v>1068572</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C46">
@@ -2780,10 +2839,10 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="10">
+      <c r="A47" s="9">
         <v>1074455</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C47">
@@ -2791,10 +2850,10 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="10">
+      <c r="A48" s="9">
         <v>1074455</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C48">
@@ -2802,10 +2861,10 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="10">
+      <c r="A49" s="9">
         <v>1058108</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C49">
@@ -2813,10 +2872,10 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="10">
+      <c r="A50" s="9">
         <v>1058108</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C50">
@@ -2824,10 +2883,10 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <v>1058108</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C51">
@@ -2978,10 +3037,10 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="10">
+      <c r="A65" s="9">
         <v>1064394</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C65">
@@ -2989,10 +3048,10 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="10">
+      <c r="A66" s="9">
         <v>1064394</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C66">
@@ -3000,10 +3059,10 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="10">
+      <c r="A67" s="9">
         <v>1062366</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C67">
@@ -3011,10 +3070,10 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="10">
+      <c r="A68" s="9">
         <v>1062366</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C68">
@@ -3022,10 +3081,10 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="10">
+      <c r="A69" s="9">
         <v>1068572</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C69">
@@ -3033,10 +3092,10 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="10">
+      <c r="A70" s="9">
         <v>1068572</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C70">
@@ -3044,10 +3103,10 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="10">
+      <c r="A71" s="9">
         <v>1068572</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C71">
@@ -3055,10 +3114,10 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="10">
+      <c r="A72" s="9">
         <v>1074455</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C72">
@@ -3066,10 +3125,10 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="10">
+      <c r="A73" s="9">
         <v>1074455</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C73">
@@ -3077,10 +3136,10 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="10">
+      <c r="A74" s="9">
         <v>1058108</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C74">
@@ -3088,10 +3147,10 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="10">
+      <c r="A75" s="9">
         <v>1058108</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C75">
@@ -3099,10 +3158,10 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="10">
+      <c r="A76" s="9">
         <v>1058108</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C76">
@@ -3110,10 +3169,10 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="13">
+      <c r="A77" s="12">
         <v>925878</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C77">
@@ -3121,10 +3180,10 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="13">
+      <c r="A78" s="12">
         <v>925878</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C78">
@@ -3132,10 +3191,10 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="13">
+      <c r="A79" s="12">
         <v>925878</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C79">
@@ -3143,10 +3202,10 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="13">
+      <c r="A80" s="12">
         <v>925878</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C80">
@@ -3154,10 +3213,10 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="13">
+      <c r="A81" s="12">
         <v>925878</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C81">
@@ -3165,10 +3224,10 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="13">
+      <c r="A82" s="12">
         <v>925878</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C82">
@@ -3184,7 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5C8D93-7AE0-4EA0-BF68-EDDEB9ED6B6E}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3313,10 +3372,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>1064394</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -3330,10 +3389,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>1062366</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -3347,10 +3406,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>1068572</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C10">
@@ -3364,10 +3423,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>1074455</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C11">
@@ -3381,10 +3440,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>1058108</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C12">
@@ -3398,10 +3457,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>925878</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C13">
@@ -3415,7 +3474,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
+      <c r="A14" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>